<commit_message>
Ejercicios Semana 25 al 29 octubre
Algoritmo de burbuja
</commit_message>
<xml_diff>
--- a/T_010_Arreglos3_NumeroMayoArreglos_EjemploPSeInt_PruebaEscritorio.xlsx
+++ b/T_010_Arreglos3_NumeroMayoArreglos_EjemploPSeInt_PruebaEscritorio.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phzro\Desktop\upbc\2021-3\Clases\introduccion a la programacion\Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9D6FAD-C1B7-4F07-87E6-C4D3D328B31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56CFEC3-CB02-42DB-9E5B-862C1A95F9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="1440" windowWidth="15375" windowHeight="10335" xr2:uid="{52D76E13-A468-41C1-A392-64BAB1497E8C}"/>
+    <workbookView xWindow="4785" yWindow="315" windowWidth="15375" windowHeight="10335" activeTab="2" xr2:uid="{52D76E13-A468-41C1-A392-64BAB1497E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ordenar" sheetId="2" r:id="rId2"/>
+    <sheet name="Ordenacion BubleSort (Burbuja)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>i</t>
   </si>
@@ -73,13 +75,143 @@
   </si>
   <si>
     <t>i=9</t>
+  </si>
+  <si>
+    <t>n=10</t>
+  </si>
+  <si>
+    <t>ArregloN</t>
+  </si>
+  <si>
+    <t>ArregloCadena</t>
+  </si>
+  <si>
+    <t>AregregloCaraceter</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>adios</t>
+  </si>
+  <si>
+    <t>pato</t>
+  </si>
+  <si>
+    <t>perro</t>
+  </si>
+  <si>
+    <t>caballo</t>
+  </si>
+  <si>
+    <t>perico</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>n=6</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>;&lt;-</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>i&lt;-i+1</t>
+  </si>
+  <si>
+    <t>mayor</t>
+  </si>
+  <si>
+    <t>Intercambio</t>
+  </si>
+  <si>
+    <t>(Swap)</t>
+  </si>
+  <si>
+    <t>ArregloN[Mayor]&gt;ArregloN[i]</t>
+  </si>
+  <si>
+    <t>arregloN[i]&lt;-arregloN[mayor]</t>
+  </si>
+  <si>
+    <t>temp&lt;-arregloN[mayor]</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>temp&lt;-arregloN[i]</t>
+  </si>
+  <si>
+    <t>arregloN[mayor]&lt;-temp</t>
+  </si>
+  <si>
+    <t>mayor&lt;-i</t>
+  </si>
+  <si>
+    <t>6&gt;4</t>
+  </si>
+  <si>
+    <t>mayor&lt;-0</t>
+  </si>
+  <si>
+    <t>i&lt;-mayor+1</t>
+  </si>
+  <si>
+    <t>i&lt;N</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>mayor+1</t>
+  </si>
+  <si>
+    <t>arregloN[mayor]&lt;-arregloN[mayor+1]</t>
+  </si>
+  <si>
+    <t>arregloN[mayor+1]&lt;-temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,8 +245,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -122,19 +266,246 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007C61D7-6450-45F6-BE6F-70BE65C466DB}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,6 +866,9 @@
       <c r="K1" s="2">
         <v>1</v>
       </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -802,4 +1176,895 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A588AA-02B8-4D78-8A55-5705E4A837E2}">
+  <dimension ref="B2:J36"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>4</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4</v>
+      </c>
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>4</v>
+      </c>
+      <c r="H14" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7">
+        <v>4</v>
+      </c>
+      <c r="H20" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7">
+        <v>2</v>
+      </c>
+      <c r="F24" s="7">
+        <v>3</v>
+      </c>
+      <c r="G24" s="7">
+        <v>4</v>
+      </c>
+      <c r="H24" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3</v>
+      </c>
+      <c r="G31" s="7">
+        <v>4</v>
+      </c>
+      <c r="H31" s="7">
+        <v>5</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3</v>
+      </c>
+      <c r="G36" s="7">
+        <v>4</v>
+      </c>
+      <c r="H36" s="7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J30:J35">
+    <sortCondition descending="1" ref="J30:J35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9D2EF-C500-4E35-958F-B48DDEBE5FEA}">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="6">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6">
+        <v>6</v>
+      </c>
+      <c r="G1" s="6">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6">
+        <v>5</v>
+      </c>
+      <c r="I1" s="6">
+        <v>4</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="12">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
+        <v>5</v>
+      </c>
+      <c r="I2" s="12">
+        <v>4</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="13">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13">
+        <v>6</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>5</v>
+      </c>
+      <c r="I3" s="13">
+        <v>4</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>6</v>
+      </c>
+      <c r="H4" s="12">
+        <v>5</v>
+      </c>
+      <c r="I4" s="12">
+        <v>4</v>
+      </c>
+      <c r="J4" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>6</v>
+      </c>
+      <c r="I5" s="12">
+        <v>4</v>
+      </c>
+      <c r="J5" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5</v>
+      </c>
+      <c r="H6" s="12">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12">
+        <v>6</v>
+      </c>
+      <c r="J6" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>5</v>
+      </c>
+      <c r="H17" s="6">
+        <v>4</v>
+      </c>
+      <c r="I17" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>3</v>
+      </c>
+      <c r="H18" s="7">
+        <v>4</v>
+      </c>
+      <c r="I18" s="7">
+        <v>5</v>
+      </c>
+      <c r="J18" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F29:H29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>